<commit_message>
ADDITION graph for 'Góc che khuất' tab pane.
</commit_message>
<xml_diff>
--- a/Document/Mặt cắt địa hình - công thức.xlsx
+++ b/Document/Mặt cắt địa hình - công thức.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -347,7 +348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -490,4 +491,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3.5</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>4.5</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>